<commit_message>
Change algorithm to bit-parallel computation. Not finished yet.
</commit_message>
<xml_diff>
--- a/examples/complete/Conway/GameRules.xlsx
+++ b/examples/complete/Conway/GameRules.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Current</t>
   </si>
@@ -103,6 +104,36 @@
   </si>
   <si>
     <t>3. if 4 ==&gt; keep current cell</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A ^ B</t>
+  </si>
+  <si>
+    <t>(A ^ B) &amp; C</t>
+  </si>
+  <si>
+    <t>A &amp; C</t>
+  </si>
+  <si>
+    <t>L = (A ^ B) ^ C</t>
+  </si>
+  <si>
+    <t>H = ((A ^ B) &amp; C) | (A &amp; C)</t>
+  </si>
+  <si>
+    <t>(A ^ B) | A</t>
+  </si>
+  <si>
+    <t>((A ^ B) | A) &amp; C</t>
   </si>
 </sst>
 </file>
@@ -126,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +167,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -181,6 +218,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +542,7 @@
   <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,4 +1291,316 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="76" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="11.42578125" style="2"/>
+    <col min="6" max="6" width="15" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="2"/>
+    <col min="10" max="10" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Conway game rules and truth tables used for bit-parallel algorithm.
</commit_message>
<xml_diff>
--- a/examples/complete/Conway/GameRules.xlsx
+++ b/examples/complete/Conway/GameRules.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Classical" sheetId="1" r:id="rId1"/>
+    <sheet name="Bit-parallel" sheetId="3" r:id="rId2"/>
+    <sheet name="Adder" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
   <si>
     <t>Current</t>
   </si>
@@ -121,19 +122,40 @@
     <t>(A ^ B) &amp; C</t>
   </si>
   <si>
-    <t>A &amp; C</t>
-  </si>
-  <si>
     <t>L = (A ^ B) ^ C</t>
   </si>
   <si>
-    <t>H = ((A ^ B) &amp; C) | (A &amp; C)</t>
-  </si>
-  <si>
-    <t>(A ^ B) | A</t>
-  </si>
-  <si>
-    <t>((A ^ B) | A) &amp; C</t>
+    <t>A &amp; B</t>
+  </si>
+  <si>
+    <t>H = ((A ^ B) &amp; C) | (A &amp; B)</t>
+  </si>
+  <si>
+    <t>total_3</t>
+  </si>
+  <si>
+    <t>total_2</t>
+  </si>
+  <si>
+    <t>total_1</t>
+  </si>
+  <si>
+    <t>total_0</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>N = all neighbours, including self</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>next</t>
   </si>
 </sst>
 </file>
@@ -157,7 +179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +195,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -222,6 +250,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,7 +573,7 @@
   </sheetPr>
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
@@ -1295,10 +1327,371 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G2" sqref="G2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,11 +1700,9 @@
     <col min="6" max="6" width="15" style="2" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" customWidth="1"/>
     <col min="8" max="8" width="15" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="2"/>
-    <col min="10" max="10" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
@@ -1328,22 +1719,16 @@
         <v>32</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>35</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1359,23 +1744,17 @@
       <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9">
         <v>0</v>
       </c>
       <c r="H2" s="4">
         <v>0</v>
       </c>
-      <c r="I2" s="4">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>0</v>
       </c>
@@ -1391,23 +1770,17 @@
       <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
         <v>0</v>
       </c>
       <c r="H3" s="4">
         <v>1</v>
       </c>
-      <c r="I3" s="4">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -1423,23 +1796,17 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
         <v>0</v>
       </c>
       <c r="H4" s="4">
         <v>1</v>
       </c>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>0</v>
       </c>
@@ -1455,23 +1822,17 @@
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
         <v>1</v>
       </c>
       <c r="H5" s="4">
         <v>0</v>
       </c>
-      <c r="I5" s="4">
-        <v>1</v>
-      </c>
-      <c r="J5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -1487,23 +1848,17 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
         <v>0</v>
       </c>
       <c r="H6" s="4">
         <v>1</v>
       </c>
-      <c r="I6" s="4">
-        <v>1</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -1519,23 +1874,17 @@
       <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="F7" s="9">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9">
         <v>1</v>
       </c>
       <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="I7" s="4">
-        <v>1</v>
-      </c>
-      <c r="J7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -1551,23 +1900,17 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
         <v>0</v>
       </c>
       <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -1583,19 +1926,13 @@
       <c r="E9" s="4">
         <v>0</v>
       </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
         <v>1</v>
       </c>
       <c r="H9" s="4">
-        <v>1</v>
-      </c>
-      <c r="I9" s="4">
-        <v>1</v>
-      </c>
-      <c r="J9" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>